<commit_message>
変更３ (reverted from commit f52028a5cfda461b5996f04bb311a2e5866f9cd4)
</commit_message>
<xml_diff>
--- a/git test.xlsx
+++ b/git test.xlsx
@@ -348,18 +348,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G16"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
-  <cols>
-    <col min="7" max="7" width="11.625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A1">
         <v>1</v>
       </c>
@@ -371,12 +368,8 @@
         <f>C1^2</f>
         <v>1</v>
       </c>
-      <c r="G1">
-        <f>E1^2</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>2</v>
       </c>
@@ -388,12 +381,8 @@
         <f t="shared" ref="E2:E16" si="1">C2^2</f>
         <v>16</v>
       </c>
-      <c r="G2">
-        <f t="shared" ref="G2:G16" si="2">E2^2</f>
-        <v>256</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>3</v>
       </c>
@@ -405,12 +394,8 @@
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-      <c r="G3">
-        <f t="shared" si="2"/>
-        <v>6561</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>4</v>
       </c>
@@ -422,12 +407,8 @@
         <f t="shared" si="1"/>
         <v>256</v>
       </c>
-      <c r="G4">
-        <f t="shared" si="2"/>
-        <v>65536</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>5</v>
       </c>
@@ -439,12 +420,8 @@
         <f t="shared" si="1"/>
         <v>625</v>
       </c>
-      <c r="G5">
-        <f t="shared" si="2"/>
-        <v>390625</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>6</v>
       </c>
@@ -456,12 +433,8 @@
         <f t="shared" si="1"/>
         <v>1296</v>
       </c>
-      <c r="G6">
-        <f t="shared" si="2"/>
-        <v>1679616</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>7</v>
       </c>
@@ -473,12 +446,8 @@
         <f t="shared" si="1"/>
         <v>2401</v>
       </c>
-      <c r="G7">
-        <f t="shared" si="2"/>
-        <v>5764801</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>8</v>
       </c>
@@ -490,12 +459,8 @@
         <f t="shared" si="1"/>
         <v>4096</v>
       </c>
-      <c r="G8">
-        <f t="shared" si="2"/>
-        <v>16777216</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>9</v>
       </c>
@@ -507,12 +472,8 @@
         <f t="shared" si="1"/>
         <v>6561</v>
       </c>
-      <c r="G9">
-        <f t="shared" si="2"/>
-        <v>43046721</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>10</v>
       </c>
@@ -524,12 +485,8 @@
         <f t="shared" si="1"/>
         <v>10000</v>
       </c>
-      <c r="G10">
-        <f t="shared" si="2"/>
-        <v>100000000</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>11</v>
       </c>
@@ -541,12 +498,8 @@
         <f t="shared" si="1"/>
         <v>14641</v>
       </c>
-      <c r="G11">
-        <f t="shared" si="2"/>
-        <v>214358881</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>12</v>
       </c>
@@ -558,12 +511,8 @@
         <f t="shared" si="1"/>
         <v>20736</v>
       </c>
-      <c r="G12">
-        <f t="shared" si="2"/>
-        <v>429981696</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>13</v>
       </c>
@@ -575,12 +524,8 @@
         <f t="shared" si="1"/>
         <v>28561</v>
       </c>
-      <c r="G13">
-        <f t="shared" si="2"/>
-        <v>815730721</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>14</v>
       </c>
@@ -592,12 +537,8 @@
         <f t="shared" si="1"/>
         <v>38416</v>
       </c>
-      <c r="G14">
-        <f t="shared" si="2"/>
-        <v>1475789056</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>15</v>
       </c>
@@ -609,12 +550,8 @@
         <f t="shared" si="1"/>
         <v>50625</v>
       </c>
-      <c r="G15">
-        <f t="shared" si="2"/>
-        <v>2562890625</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>16</v>
       </c>
@@ -625,10 +562,6 @@
       <c r="E16">
         <f t="shared" si="1"/>
         <v>65536</v>
-      </c>
-      <c r="G16">
-        <f t="shared" si="2"/>
-        <v>4294967296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
変更３ (reverted from commit f52028a5cfda461b5996f04bb311a2e5866f9cd4) (reverted from commit 4da27d3fc190dcc8bb9a5f1c2093dcef964bf4d9)
</commit_message>
<xml_diff>
--- a/git test.xlsx
+++ b/git test.xlsx
@@ -348,15 +348,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E16"/>
+  <dimension ref="A1:G16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.4"/>
+  <cols>
+    <col min="7" max="7" width="11.625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1">
         <v>1</v>
       </c>
@@ -368,8 +371,12 @@
         <f>C1^2</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G1">
+        <f>E1^2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2">
         <v>2</v>
       </c>
@@ -381,8 +388,12 @@
         <f t="shared" ref="E2:E16" si="1">C2^2</f>
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G2">
+        <f t="shared" ref="G2:G16" si="2">E2^2</f>
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3">
         <v>3</v>
       </c>
@@ -394,8 +405,12 @@
         <f t="shared" si="1"/>
         <v>81</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G3">
+        <f t="shared" si="2"/>
+        <v>6561</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4">
         <v>4</v>
       </c>
@@ -407,8 +422,12 @@
         <f t="shared" si="1"/>
         <v>256</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G4">
+        <f t="shared" si="2"/>
+        <v>65536</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5">
         <v>5</v>
       </c>
@@ -420,8 +439,12 @@
         <f t="shared" si="1"/>
         <v>625</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G5">
+        <f t="shared" si="2"/>
+        <v>390625</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6">
         <v>6</v>
       </c>
@@ -433,8 +456,12 @@
         <f t="shared" si="1"/>
         <v>1296</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G6">
+        <f t="shared" si="2"/>
+        <v>1679616</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7">
         <v>7</v>
       </c>
@@ -446,8 +473,12 @@
         <f t="shared" si="1"/>
         <v>2401</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G7">
+        <f t="shared" si="2"/>
+        <v>5764801</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8">
         <v>8</v>
       </c>
@@ -459,8 +490,12 @@
         <f t="shared" si="1"/>
         <v>4096</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G8">
+        <f t="shared" si="2"/>
+        <v>16777216</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9">
         <v>9</v>
       </c>
@@ -472,8 +507,12 @@
         <f t="shared" si="1"/>
         <v>6561</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G9">
+        <f t="shared" si="2"/>
+        <v>43046721</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A10">
         <v>10</v>
       </c>
@@ -485,8 +524,12 @@
         <f t="shared" si="1"/>
         <v>10000</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G10">
+        <f t="shared" si="2"/>
+        <v>100000000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11">
         <v>11</v>
       </c>
@@ -498,8 +541,12 @@
         <f t="shared" si="1"/>
         <v>14641</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G11">
+        <f t="shared" si="2"/>
+        <v>214358881</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12">
         <v>12</v>
       </c>
@@ -511,8 +558,12 @@
         <f t="shared" si="1"/>
         <v>20736</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G12">
+        <f t="shared" si="2"/>
+        <v>429981696</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A13">
         <v>13</v>
       </c>
@@ -524,8 +575,12 @@
         <f t="shared" si="1"/>
         <v>28561</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G13">
+        <f t="shared" si="2"/>
+        <v>815730721</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A14">
         <v>14</v>
       </c>
@@ -537,8 +592,12 @@
         <f t="shared" si="1"/>
         <v>38416</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G14">
+        <f t="shared" si="2"/>
+        <v>1475789056</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A15">
         <v>15</v>
       </c>
@@ -550,8 +609,12 @@
         <f t="shared" si="1"/>
         <v>50625</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="G15">
+        <f t="shared" si="2"/>
+        <v>2562890625</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A16">
         <v>16</v>
       </c>
@@ -562,6 +625,10 @@
       <c r="E16">
         <f t="shared" si="1"/>
         <v>65536</v>
+      </c>
+      <c r="G16">
+        <f t="shared" si="2"/>
+        <v>4294967296</v>
       </c>
     </row>
   </sheetData>

</xml_diff>